<commit_message>
Add generation file and TD
</commit_message>
<xml_diff>
--- a/Данные_на_проверку.xlsx
+++ b/Данные_на_проверку.xlsx
@@ -736,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1248,13 +1248,13 @@
         <v>77</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>24</v>
       </c>
       <c r="E18" s="4">
-        <v>3999</v>
+        <v>3634</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>17</v>

</xml_diff>